<commit_message>
feat: :sparkles: Agregando masterplan
</commit_message>
<xml_diff>
--- a/database/seeders/lotificacions.xlsx
+++ b/database/seeders/lotificacions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="22">
   <si>
     <t>etapa</t>
   </si>
@@ -1228,10 +1228,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q1000"/>
+  <dimension ref="A1:Q1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6333333333333" defaultRowHeight="15" customHeight="1"/>
@@ -1440,7 +1440,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="2">
-        <f>(H4*0.15)</f>
+        <f t="shared" si="0"/>
         <v>11250</v>
       </c>
       <c r="K4" s="2">
@@ -4062,7 +4062,7 @@
         <v>2</v>
       </c>
       <c r="B53" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>17</v>
@@ -4116,7 +4116,7 @@
         <v>2</v>
       </c>
       <c r="B54" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>17</v>
@@ -4134,14 +4134,14 @@
         <v>260</v>
       </c>
       <c r="H54" s="3">
-        <v>78000</v>
+        <v>75000</v>
       </c>
       <c r="I54" s="4">
         <v>1</v>
       </c>
       <c r="J54" s="2">
-        <f t="shared" si="0"/>
-        <v>11700</v>
+        <f>(H54*0.15)</f>
+        <v>11250</v>
       </c>
       <c r="K54" s="2">
         <v>953.3333333</v>
@@ -4165,7 +4165,60 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1" spans="1:17">
+      <c r="A55" s="2">
+        <v>2</v>
+      </c>
+      <c r="B55" s="2">
+        <v>276</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="2">
+        <v>10</v>
+      </c>
+      <c r="E55" s="2">
+        <v>20</v>
+      </c>
+      <c r="F55" s="2">
+        <v>200</v>
+      </c>
+      <c r="G55" s="2">
+        <v>260</v>
+      </c>
+      <c r="H55" s="3">
+        <v>78000</v>
+      </c>
+      <c r="I55" s="4">
+        <v>1</v>
+      </c>
+      <c r="J55" s="2">
+        <f>(H55*0.15)</f>
+        <v>11700</v>
+      </c>
+      <c r="K55" s="2">
+        <v>953.3333333</v>
+      </c>
+      <c r="L55" s="2">
+        <v>1271.111111</v>
+      </c>
+      <c r="M55" s="2">
+        <v>1906.666667</v>
+      </c>
+      <c r="N55" s="2">
+        <v>3813.333333</v>
+      </c>
+      <c r="O55" s="2">
+        <v>7626.666667</v>
+      </c>
+      <c r="P55" s="2">
+        <v>46800</v>
+      </c>
+      <c r="Q55" s="3">
+        <v>1000</v>
+      </c>
+    </row>
     <row r="56" ht="15.75" customHeight="1"/>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1"/>
@@ -5111,6 +5164,7 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="1" orientation="landscape"/>

</xml_diff>